<commit_message>
xong moi chuc nang co ban
</commit_message>
<xml_diff>
--- a/public/mau.xlsx
+++ b/public/mau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lap Trinh\NodeJs\BocThamVongTron\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FF385D-F702-44D3-86C4-525746F9943A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56F6F6D-BC00-424E-AA15-B118B5DA5E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24C2CB95-7022-49C4-B371-12CE8A8138D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>STT</t>
   </si>
@@ -89,7 +89,7 @@
     <t>Chim Sẻ Đi Nắng</t>
   </si>
   <si>
-    <t>Đế Chế</t>
+    <t>HCM</t>
   </si>
 </sst>
 </file>
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1B2A19-02D0-409B-ADA0-EF63FDFFA6FD}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -605,140 +605,38 @@
         <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>